<commit_message>
Updated item report and return with SQL
Added functionality of report and return and linked with SQL database
Minor fixes
</commit_message>
<xml_diff>
--- a/Front End/eo.xlsx
+++ b/Front End/eo.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingwen.hu/Documents/GitHub/KeyShare/keyshare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jingwen.hu/Documents/GitHub/KeyShare/Front End/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C907E97-8D85-DC42-8E25-E9210C1DDC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46285192-7ADC-B348-AB9D-20FAB5A81AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{C7993506-B2B5-7841-8514-E5A3A8F0853E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,12 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>a32</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>a3</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b3</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -413,25 +440,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{927092E7-A33E-9A4F-97F0-1C8944709EE3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>